<commit_message>
Cuối cùng thì đã biết Lớp này học môn nào vào Học kỳ nào
</commit_message>
<xml_diff>
--- a/Tài liệu/Chuongtrinhdaotao_Dât.xlsx
+++ b/Tài liệu/Chuongtrinhdaotao_Dât.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BAI TAP\Đồ Án Nghiên Cứu khoa Học 2024\Application-Managing-and-Optimizing-Faculty-Teaching-Hours\Tài liệu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\CN\CN_Backup\Tài liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FFBB3E-0063-4C6E-AA72-0DE11117FDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C81818-CEC7-475E-A25D-2651055551D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -959,7 +959,7 @@
       <charset val="163"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -969,6 +969,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFEF2CB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1000,7 +1006,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1041,8 +1047,8 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1050,8 +1056,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1335,28 +1359,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A322" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F344" sqref="F344"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E71" sqref="E67:E71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="109.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="48.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.6640625" style="1"/>
+    <col min="3" max="3" width="26.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="109.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
@@ -1393,13 +1417,13 @@
       <c r="L1" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-    </row>
-    <row r="2" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+    </row>
+    <row r="2" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1412,13 +1436,13 @@
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-    </row>
-    <row r="3" spans="1:17" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+    </row>
+    <row r="3" spans="1:17" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>70</v>
       </c>
@@ -1456,7 +1480,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1494,7 +1518,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1532,7 +1556,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1570,7 +1594,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1608,7 +1632,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>280</v>
       </c>
@@ -1646,7 +1670,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1684,7 +1708,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -1722,7 +1746,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1760,7 +1784,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -1798,7 +1822,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -1836,7 +1860,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -1874,7 +1898,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>276</v>
       </c>
@@ -1912,7 +1936,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1950,7 +1974,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
@@ -1988,7 +2012,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -2026,7 +2050,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -2064,7 +2088,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
@@ -2102,7 +2126,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -2140,7 +2164,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
@@ -2178,7 +2202,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
@@ -2216,7 +2240,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
@@ -2254,7 +2278,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
@@ -2292,7 +2316,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -2330,7 +2354,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>29</v>
       </c>
@@ -2368,7 +2392,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>30</v>
       </c>
@@ -2406,7 +2430,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>31</v>
       </c>
@@ -2444,7 +2468,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>32</v>
       </c>
@@ -2482,7 +2506,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
@@ -2520,7 +2544,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>34</v>
       </c>
@@ -2558,7 +2582,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>35</v>
       </c>
@@ -2596,7 +2620,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>284</v>
       </c>
@@ -2634,7 +2658,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>36</v>
       </c>
@@ -2672,7 +2696,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
@@ -2710,7 +2734,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>38</v>
       </c>
@@ -2748,7 +2772,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>39</v>
       </c>
@@ -2786,7 +2810,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>285</v>
       </c>
@@ -2824,7 +2848,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
@@ -2862,7 +2886,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -2900,7 +2924,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -2938,7 +2962,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>275</v>
       </c>
@@ -2976,7 +3000,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>278</v>
       </c>
@@ -3014,7 +3038,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
@@ -3052,7 +3076,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>44</v>
       </c>
@@ -3090,7 +3114,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>277</v>
       </c>
@@ -3128,7 +3152,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>45</v>
       </c>
@@ -3166,7 +3190,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>46</v>
       </c>
@@ -3204,7 +3228,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>47</v>
       </c>
@@ -3242,7 +3266,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>48</v>
       </c>
@@ -3280,7 +3304,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>279</v>
       </c>
@@ -3318,7 +3342,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>49</v>
       </c>
@@ -3356,7 +3380,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>50</v>
       </c>
@@ -3394,7 +3418,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>51</v>
       </c>
@@ -3432,7 +3456,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>52</v>
       </c>
@@ -3470,7 +3494,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>53</v>
       </c>
@@ -3508,7 +3532,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>54</v>
       </c>
@@ -3546,7 +3570,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="19.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>283</v>
       </c>
@@ -3584,7 +3608,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
         <v>281</v>
       </c>
@@ -3622,7 +3646,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>55</v>
       </c>
@@ -3660,7 +3684,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>56</v>
       </c>
@@ -3698,7 +3722,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>57</v>
       </c>
@@ -3736,7 +3760,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>58</v>
       </c>
@@ -3774,7 +3798,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
         <v>282</v>
       </c>
@@ -3812,7 +3836,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>59</v>
       </c>
@@ -3850,7 +3874,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>60</v>
       </c>
@@ -3888,7 +3912,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>61</v>
       </c>
@@ -3926,7 +3950,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>62</v>
       </c>
@@ -3964,7 +3988,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>273</v>
       </c>
@@ -4002,7 +4026,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>274</v>
       </c>
@@ -4040,45 +4064,45 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
+    <row r="72" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="18">
         <v>5</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72" s="18">
         <v>5</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="18">
         <v>0</v>
       </c>
-      <c r="E72" s="8">
-        <v>1</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H72" s="6" t="s">
+      <c r="E72" s="19">
+        <v>1</v>
+      </c>
+      <c r="F72" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="G72" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H72" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="I72" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J72" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="K72" s="6">
-        <v>140</v>
-      </c>
-      <c r="L72" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I72" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="J72" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="K72" s="22">
+        <v>140</v>
+      </c>
+      <c r="L72" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>77</v>
       </c>
@@ -4116,7 +4140,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>78</v>
       </c>
@@ -4154,7 +4178,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>18</v>
       </c>
@@ -4192,7 +4216,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>79</v>
       </c>
@@ -4230,7 +4254,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>80</v>
       </c>
@@ -4268,7 +4292,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>19</v>
       </c>
@@ -4306,7 +4330,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>81</v>
       </c>
@@ -4344,7 +4368,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>82</v>
       </c>
@@ -4382,7 +4406,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>83</v>
       </c>
@@ -4420,7 +4444,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
@@ -4458,7 +4482,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>39</v>
       </c>
@@ -4496,7 +4520,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>84</v>
       </c>
@@ -4534,7 +4558,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>85</v>
       </c>
@@ -4572,7 +4596,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>86</v>
       </c>
@@ -4610,7 +4634,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>87</v>
       </c>
@@ -4648,7 +4672,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>88</v>
       </c>
@@ -4686,7 +4710,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>89</v>
       </c>
@@ -4724,7 +4748,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>5</v>
       </c>
@@ -4762,7 +4786,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>90</v>
       </c>
@@ -4800,7 +4824,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>91</v>
       </c>
@@ -4838,7 +4862,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>92</v>
       </c>
@@ -4876,7 +4900,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>93</v>
       </c>
@@ -4914,7 +4938,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>94</v>
       </c>
@@ -4952,7 +4976,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>25</v>
       </c>
@@ -4990,7 +5014,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>95</v>
       </c>
@@ -5028,7 +5052,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>21</v>
       </c>
@@ -5066,7 +5090,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>96</v>
       </c>
@@ -5104,7 +5128,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>97</v>
       </c>
@@ -5142,7 +5166,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>98</v>
       </c>
@@ -5180,7 +5204,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>52</v>
       </c>
@@ -5218,7 +5242,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>99</v>
       </c>
@@ -5256,7 +5280,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>100</v>
       </c>
@@ -5294,7 +5318,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>101</v>
       </c>
@@ -5332,7 +5356,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>102</v>
       </c>
@@ -5370,7 +5394,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>103</v>
       </c>
@@ -5408,7 +5432,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>104</v>
       </c>
@@ -5446,7 +5470,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>105</v>
       </c>
@@ -5484,7 +5508,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>106</v>
       </c>
@@ -5522,7 +5546,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>107</v>
       </c>
@@ -5560,7 +5584,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>108</v>
       </c>
@@ -5598,7 +5622,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>109</v>
       </c>
@@ -5636,7 +5660,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>110</v>
       </c>
@@ -5674,7 +5698,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>111</v>
       </c>
@@ -5712,7 +5736,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>22</v>
       </c>
@@ -5750,7 +5774,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>112</v>
       </c>
@@ -5788,7 +5812,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>113</v>
       </c>
@@ -5826,7 +5850,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>114</v>
       </c>
@@ -5864,7 +5888,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>115</v>
       </c>
@@ -5902,7 +5926,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>116</v>
       </c>
@@ -5940,7 +5964,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>117</v>
       </c>
@@ -5978,7 +6002,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>118</v>
       </c>
@@ -6016,7 +6040,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>119</v>
       </c>
@@ -6054,7 +6078,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>120</v>
       </c>
@@ -6092,7 +6116,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>121</v>
       </c>
@@ -6130,7 +6154,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>122</v>
       </c>
@@ -6168,7 +6192,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>123</v>
       </c>
@@ -6206,7 +6230,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>124</v>
       </c>
@@ -6244,7 +6268,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>125</v>
       </c>
@@ -6282,7 +6306,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>126</v>
       </c>
@@ -6320,7 +6344,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>127</v>
       </c>
@@ -6358,7 +6382,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>128</v>
       </c>
@@ -6396,7 +6420,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>129</v>
       </c>
@@ -6434,7 +6458,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>130</v>
       </c>
@@ -6472,7 +6496,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>131</v>
       </c>
@@ -6510,7 +6534,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>132</v>
       </c>
@@ -6548,7 +6572,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>133</v>
       </c>
@@ -6586,7 +6610,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>134</v>
       </c>
@@ -6624,7 +6648,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>135</v>
       </c>
@@ -6662,7 +6686,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>136</v>
       </c>
@@ -6700,7 +6724,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>137</v>
       </c>
@@ -6738,7 +6762,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>138</v>
       </c>
@@ -6776,7 +6800,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>139</v>
       </c>
@@ -6814,7 +6838,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>140</v>
       </c>
@@ -6852,7 +6876,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>141</v>
       </c>
@@ -6890,7 +6914,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>142</v>
       </c>
@@ -6928,7 +6952,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>143</v>
       </c>
@@ -6966,7 +6990,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>61</v>
       </c>
@@ -7004,7 +7028,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>144</v>
       </c>
@@ -7042,7 +7066,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>145</v>
       </c>
@@ -7080,7 +7104,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>146</v>
       </c>
@@ -7118,7 +7142,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>147</v>
       </c>
@@ -7156,7 +7180,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>76</v>
       </c>
@@ -7194,7 +7218,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>77</v>
       </c>
@@ -7232,7 +7256,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>70</v>
       </c>
@@ -7270,7 +7294,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>18</v>
       </c>
@@ -7308,7 +7332,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>79</v>
       </c>
@@ -7346,7 +7370,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>80</v>
       </c>
@@ -7384,7 +7408,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>19</v>
       </c>
@@ -7422,7 +7446,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>81</v>
       </c>
@@ -7460,7 +7484,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>82</v>
       </c>
@@ -7498,7 +7522,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>83</v>
       </c>
@@ -7536,7 +7560,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>3</v>
       </c>
@@ -7574,7 +7598,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>39</v>
       </c>
@@ -7612,7 +7636,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>84</v>
       </c>
@@ -7650,7 +7674,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>85</v>
       </c>
@@ -7688,7 +7712,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>86</v>
       </c>
@@ -7726,7 +7750,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>87</v>
       </c>
@@ -7764,7 +7788,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>152</v>
       </c>
@@ -7802,7 +7826,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>89</v>
       </c>
@@ -7840,7 +7864,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>5</v>
       </c>
@@ -7878,7 +7902,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>90</v>
       </c>
@@ -7916,7 +7940,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>91</v>
       </c>
@@ -7954,7 +7978,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>92</v>
       </c>
@@ -7992,7 +8016,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>93</v>
       </c>
@@ -8030,7 +8054,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
         <v>94</v>
       </c>
@@ -8068,7 +8092,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>25</v>
       </c>
@@ -8106,7 +8130,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
         <v>95</v>
       </c>
@@ -8144,7 +8168,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
         <v>21</v>
       </c>
@@ -8182,7 +8206,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
         <v>96</v>
       </c>
@@ -8220,7 +8244,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>97</v>
       </c>
@@ -8258,7 +8282,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>98</v>
       </c>
@@ -8296,7 +8320,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
         <v>52</v>
       </c>
@@ -8334,7 +8358,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
         <v>99</v>
       </c>
@@ -8372,7 +8396,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
         <v>100</v>
       </c>
@@ -8410,7 +8434,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
         <v>101</v>
       </c>
@@ -8448,7 +8472,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>102</v>
       </c>
@@ -8486,7 +8510,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
         <v>103</v>
       </c>
@@ -8524,7 +8548,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
         <v>104</v>
       </c>
@@ -8562,7 +8586,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>105</v>
       </c>
@@ -8600,7 +8624,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
         <v>106</v>
       </c>
@@ -8638,7 +8662,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>107</v>
       </c>
@@ -8676,7 +8700,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>108</v>
       </c>
@@ -8714,7 +8738,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>109</v>
       </c>
@@ -8752,7 +8776,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>153</v>
       </c>
@@ -8790,7 +8814,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>22</v>
       </c>
@@ -8828,7 +8852,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>112</v>
       </c>
@@ -8866,7 +8890,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>113</v>
       </c>
@@ -8904,7 +8928,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
         <v>154</v>
       </c>
@@ -8942,7 +8966,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>111</v>
       </c>
@@ -8980,7 +9004,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>155</v>
       </c>
@@ -9018,7 +9042,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>156</v>
       </c>
@@ -9056,7 +9080,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
         <v>157</v>
       </c>
@@ -9094,7 +9118,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>158</v>
       </c>
@@ -9132,7 +9156,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>159</v>
       </c>
@@ -9170,7 +9194,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>160</v>
       </c>
@@ -9208,7 +9232,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>161</v>
       </c>
@@ -9246,7 +9270,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>162</v>
       </c>
@@ -9284,7 +9308,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>163</v>
       </c>
@@ -9322,7 +9346,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211" s="3" t="s">
         <v>123</v>
       </c>
@@ -9360,7 +9384,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
         <v>164</v>
       </c>
@@ -9398,7 +9422,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>165</v>
       </c>
@@ -9436,7 +9460,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
         <v>166</v>
       </c>
@@ -9474,7 +9498,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>167</v>
       </c>
@@ -9512,7 +9536,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
         <v>168</v>
       </c>
@@ -9550,7 +9574,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>169</v>
       </c>
@@ -9588,7 +9612,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
         <v>119</v>
       </c>
@@ -9626,7 +9650,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>170</v>
       </c>
@@ -9664,7 +9688,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220" s="3" t="s">
         <v>171</v>
       </c>
@@ -9702,7 +9726,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" s="3" t="s">
         <v>172</v>
       </c>
@@ -9740,7 +9764,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>173</v>
       </c>
@@ -9778,7 +9802,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223" s="3" t="s">
         <v>174</v>
       </c>
@@ -9816,7 +9840,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" s="3" t="s">
         <v>175</v>
       </c>
@@ -9854,7 +9878,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
         <v>176</v>
       </c>
@@ -9892,7 +9916,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226" s="3" t="s">
         <v>177</v>
       </c>
@@ -9930,7 +9954,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
         <v>178</v>
       </c>
@@ -9968,7 +9992,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
         <v>137</v>
       </c>
@@ -10006,7 +10030,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
         <v>179</v>
       </c>
@@ -10044,7 +10068,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230" s="3" t="s">
         <v>180</v>
       </c>
@@ -10082,7 +10106,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>181</v>
       </c>
@@ -10120,7 +10144,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
         <v>182</v>
       </c>
@@ -10158,7 +10182,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233" s="3" t="s">
         <v>183</v>
       </c>
@@ -10196,7 +10220,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234" s="3" t="s">
         <v>61</v>
       </c>
@@ -10234,7 +10258,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235" s="3" t="s">
         <v>144</v>
       </c>
@@ -10272,7 +10296,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
         <v>184</v>
       </c>
@@ -10310,7 +10334,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
         <v>185</v>
       </c>
@@ -10348,7 +10372,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
         <v>186</v>
       </c>
@@ -10386,7 +10410,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
         <v>187</v>
       </c>
@@ -10424,7 +10448,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" s="10" t="s">
         <v>191</v>
       </c>
@@ -10462,7 +10486,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
         <v>70</v>
       </c>
@@ -10500,7 +10524,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242" s="10" t="s">
         <v>194</v>
       </c>
@@ -10538,7 +10562,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243" s="10" t="s">
         <v>196</v>
       </c>
@@ -10576,7 +10600,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244" s="10" t="s">
         <v>199</v>
       </c>
@@ -10614,7 +10638,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245" s="10" t="s">
         <v>201</v>
       </c>
@@ -10652,7 +10676,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246" s="10" t="s">
         <v>202</v>
       </c>
@@ -10690,7 +10714,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247" s="10" t="s">
         <v>203</v>
       </c>
@@ -10728,7 +10752,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248" s="10" t="s">
         <v>204</v>
       </c>
@@ -10766,7 +10790,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249" s="10" t="s">
         <v>205</v>
       </c>
@@ -10804,7 +10828,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250" s="10" t="s">
         <v>206</v>
       </c>
@@ -10842,7 +10866,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251" s="10" t="s">
         <v>207</v>
       </c>
@@ -10880,7 +10904,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252" s="10" t="s">
         <v>208</v>
       </c>
@@ -10918,7 +10942,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253" s="10" t="s">
         <v>209</v>
       </c>
@@ -10956,7 +10980,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A254" s="10" t="s">
         <v>210</v>
       </c>
@@ -10994,7 +11018,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A255" s="10" t="s">
         <v>211</v>
       </c>
@@ -11032,7 +11056,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A256" s="10" t="s">
         <v>212</v>
       </c>
@@ -11070,7 +11094,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A257" s="10" t="s">
         <v>213</v>
       </c>
@@ -11108,7 +11132,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A258" s="10" t="s">
         <v>214</v>
       </c>
@@ -11146,7 +11170,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A259" s="10" t="s">
         <v>215</v>
       </c>
@@ -11184,7 +11208,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A260" s="10" t="s">
         <v>216</v>
       </c>
@@ -11222,7 +11246,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A261" s="10" t="s">
         <v>217</v>
       </c>
@@ -11260,7 +11284,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262" s="10" t="s">
         <v>218</v>
       </c>
@@ -11298,7 +11322,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A263" s="10" t="s">
         <v>219</v>
       </c>
@@ -11336,7 +11360,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A264" s="10" t="s">
         <v>220</v>
       </c>
@@ -11374,7 +11398,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A265" s="10" t="s">
         <v>221</v>
       </c>
@@ -11412,7 +11436,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A266" s="10" t="s">
         <v>222</v>
       </c>
@@ -11450,7 +11474,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A267" s="10" t="s">
         <v>223</v>
       </c>
@@ -11488,7 +11512,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A268" s="10" t="s">
         <v>224</v>
       </c>
@@ -11526,7 +11550,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A269" s="10" t="s">
         <v>225</v>
       </c>
@@ -11564,7 +11588,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A270" s="10" t="s">
         <v>226</v>
       </c>
@@ -11602,7 +11626,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A271" s="10" t="s">
         <v>227</v>
       </c>
@@ -11640,7 +11664,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A272" s="10" t="s">
         <v>228</v>
       </c>
@@ -11678,7 +11702,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A273" s="10" t="s">
         <v>229</v>
       </c>
@@ -11716,7 +11740,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A274" s="10" t="s">
         <v>230</v>
       </c>
@@ -11754,7 +11778,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A275" s="10" t="s">
         <v>231</v>
       </c>
@@ -11792,7 +11816,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A276" s="10" t="s">
         <v>232</v>
       </c>
@@ -11830,7 +11854,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A277" s="10" t="s">
         <v>233</v>
       </c>
@@ -11868,7 +11892,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A278" s="10" t="s">
         <v>234</v>
       </c>
@@ -11906,7 +11930,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A279" s="10" t="s">
         <v>235</v>
       </c>
@@ -11944,7 +11968,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A280" s="10" t="s">
         <v>236</v>
       </c>
@@ -11982,7 +12006,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A281" s="10" t="s">
         <v>237</v>
       </c>
@@ -12020,7 +12044,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A282" s="10" t="s">
         <v>238</v>
       </c>
@@ -12058,7 +12082,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A283" s="10" t="s">
         <v>239</v>
       </c>
@@ -12096,7 +12120,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A284" s="10" t="s">
         <v>240</v>
       </c>
@@ -12134,7 +12158,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A285" s="10" t="s">
         <v>241</v>
       </c>
@@ -12172,7 +12196,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A286" s="10" t="s">
         <v>242</v>
       </c>
@@ -12210,7 +12234,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A287" s="10" t="s">
         <v>243</v>
       </c>
@@ -12248,7 +12272,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A288" s="10" t="s">
         <v>244</v>
       </c>
@@ -12286,7 +12310,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A289" s="10" t="s">
         <v>245</v>
       </c>
@@ -12324,7 +12348,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A290" s="10" t="s">
         <v>246</v>
       </c>
@@ -12362,7 +12386,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A291" s="10" t="s">
         <v>247</v>
       </c>
@@ -12400,7 +12424,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A292" s="10" t="s">
         <v>248</v>
       </c>
@@ -12438,7 +12462,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A293" s="10" t="s">
         <v>249</v>
       </c>
@@ -12476,7 +12500,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A294" s="10" t="s">
         <v>250</v>
       </c>
@@ -12514,7 +12538,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A295" s="10" t="s">
         <v>251</v>
       </c>
@@ -12552,7 +12576,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A296" s="10" t="s">
         <v>252</v>
       </c>
@@ -12590,7 +12614,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A297" s="10" t="s">
         <v>253</v>
       </c>
@@ -12628,7 +12652,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A298" s="10" t="s">
         <v>254</v>
       </c>
@@ -12666,7 +12690,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A299" s="10" t="s">
         <v>255</v>
       </c>
@@ -12704,7 +12728,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A300" s="10" t="s">
         <v>256</v>
       </c>
@@ -12742,7 +12766,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A301" s="10" t="s">
         <v>257</v>
       </c>
@@ -12780,7 +12804,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A302" s="10" t="s">
         <v>258</v>
       </c>
@@ -12818,7 +12842,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A303" s="10" t="s">
         <v>259</v>
       </c>
@@ -12856,7 +12880,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A304" s="10" t="s">
         <v>260</v>
       </c>
@@ -12894,7 +12918,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A305" s="10" t="s">
         <v>261</v>
       </c>
@@ -12932,7 +12956,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A306" s="10" t="s">
         <v>262</v>
       </c>
@@ -12970,7 +12994,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A307" s="10" t="s">
         <v>263</v>
       </c>
@@ -13008,7 +13032,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A308" s="10" t="s">
         <v>264</v>
       </c>
@@ -13046,7 +13070,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A309" s="10" t="s">
         <v>265</v>
       </c>
@@ -13084,7 +13108,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A310" s="10" t="s">
         <v>266</v>
       </c>
@@ -13122,7 +13146,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A311" s="10" t="s">
         <v>267</v>
       </c>
@@ -13160,7 +13184,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A312" s="10" t="s">
         <v>268</v>
       </c>
@@ -13198,7 +13222,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A313" s="10" t="s">
         <v>269</v>
       </c>
@@ -13236,7 +13260,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A314" s="10" t="s">
         <v>270</v>
       </c>
@@ -13274,7 +13298,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A315" s="10" t="s">
         <v>271</v>
       </c>
@@ -13312,7 +13336,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A316" s="10" t="s">
         <v>272</v>
       </c>
@@ -13350,14 +13374,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A317" s="10" t="s">
         <v>144</v>
       </c>
       <c r="B317" s="10">
         <v>7</v>
       </c>
-      <c r="C317" s="17">
+      <c r="C317" s="14">
         <v>0</v>
       </c>
       <c r="D317" s="10">
@@ -13388,7 +13412,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A318" s="10" t="s">
         <v>286</v>
       </c>
@@ -13426,7 +13450,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A319" s="10" t="s">
         <v>287</v>
       </c>
@@ -13436,7 +13460,7 @@
       <c r="C319" s="10">
         <v>4</v>
       </c>
-      <c r="D319" s="17">
+      <c r="D319" s="14">
         <v>0</v>
       </c>
       <c r="E319" s="4">
@@ -13466,12 +13490,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
@@ -13483,6 +13501,12 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>